<commit_message>
one must have hope
eyeballed the ethernet transmission lines, i think it'll work. absolute pain without using footprints smaller than 0805 but it think itll be fine. also shuffled together the PWM sig bank
</commit_message>
<xml_diff>
--- a/hardware/MasterBoard_A/Meta.xlsx
+++ b/hardware/MasterBoard_A/Meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\BeeMS\hardware\MasterBoard_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF7DDA7-960D-4528-91C4-8E7C51CD7805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98333C02-14D0-4F61-B223-63F98603464A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{E16E688C-64E3-4955-9FD3-F7092625115C}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="116">
   <si>
     <t>last updated</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>interrupt</t>
+  </si>
+  <si>
+    <t>controller CS</t>
   </si>
 </sst>
 </file>
@@ -622,11 +625,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -636,29 +636,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -681,6 +660,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,14 +689,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1032,1196 +1032,1205 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4533B8-A771-42AD-BF13-358F348FDA0F}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="14" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="3" customWidth="1"/>
-    <col min="9" max="12" width="9.140625" style="3"/>
-    <col min="13" max="13" width="13.42578125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="9" max="12" width="9.140625" style="2"/>
+    <col min="13" max="13" width="13.42578125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="3">
         <v>46011</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="G1" s="3" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="G1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="2" t="str">
+      <c r="M2" s="1" t="str">
         <f>IFERROR(INDEX($H$15:$H$1000, MATCH($L2, $G$15:$G$1000, 0)), "n/a")</f>
         <v>n/a</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="L3" s="2" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="2" t="str">
+      <c r="M3" s="1" t="str">
         <f t="shared" ref="M3:M34" si="0">IFERROR(INDEX($H$15:$H$1000, MATCH($L3, $G$15:$G$1000, 0)), "n/a")</f>
         <v>n/a</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="L4" s="2" t="s">
+      <c r="H4" s="18"/>
+      <c r="L4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="2" t="str">
+      <c r="M4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="2" t="str">
+      <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="L6" s="2" t="s">
+      <c r="H6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="2" t="str">
+      <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="L7" s="2" t="s">
+      <c r="H7" s="1"/>
+      <c r="L7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="2" t="str">
+      <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="L8" s="2" t="s">
+      <c r="H8" s="1"/>
+      <c r="L8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="2" t="str">
+      <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="L9" s="2" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="L9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M9" s="2" t="str">
+      <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="L10" s="2" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="2" t="str">
+      <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="L11" s="2" t="s">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="L11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="2" t="str">
+      <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="L12" s="2" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="L12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M12" s="2" t="str">
+      <c r="M12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="L13" s="2" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="L13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="2" t="str">
+      <c r="M13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="L14" s="2" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="L14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M14" s="2" t="str">
+      <c r="M14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>spi0 SCLK</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M15" s="2" t="str">
+      <c r="M15" s="1" t="str">
         <f>IFERROR(INDEX($H$15:$H$1000, MATCH($L15, $G$15:$G$1000, 0)), "n/a")</f>
         <v>spi0 MISO/POCI</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L16" s="2" t="s">
+      <c r="L16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M16" s="2" t="str">
+      <c r="M16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>spi0 MOSI/PICO</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="L17" s="2" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="L17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M17" s="2" t="str">
+      <c r="M17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="17" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="L18" s="2" t="s">
+      <c r="H18" s="11"/>
+      <c r="L18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="2" t="str">
+      <c r="M18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>spi1 MISO/POCI</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="7" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M19" s="2" t="str">
+      <c r="M19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>spi1 SCLK</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="2" t="s">
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="L20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M20" s="2" t="str">
+      <c r="M20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>spi1 MOSI/PICO</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="2" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="L21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M21" s="2" t="str">
+      <c r="M21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SWDIO</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="2" t="s">
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M22" s="2" t="str">
+      <c r="M22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SWCLK</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="2" t="s">
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M23" s="2" t="str">
+      <c r="M23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="2" t="s">
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M24" s="2" t="str">
+      <c r="M24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="2" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M25" s="2" t="str">
+      <c r="M25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="2" t="s">
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M26" s="2" t="str">
+      <c r="M26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="2" t="s">
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M27" s="2" t="str">
+      <c r="M27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="2" t="s">
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="L28" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M28" s="2" t="str">
+      <c r="M28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MCAN0 TX</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="L29" s="2" t="s">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="L29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M29" s="2" t="str">
+      <c r="M29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>MCAN0 RX</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L30" s="2" t="s">
+      <c r="L30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M30" s="2" t="str">
+      <c r="M30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M31" s="2" t="str">
+      <c r="M31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="L32" s="2" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="L32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M32" s="2" t="str">
+      <c r="M32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="1" t="s">
+      <c r="F33" s="15"/>
+      <c r="G33" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="L33" s="2" t="s">
+      <c r="H33" s="18"/>
+      <c r="L33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M33" s="2" t="str">
+      <c r="M33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>n/a</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="7" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="L34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M34" s="3" t="str">
+      <c r="M34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>gpio</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="8"/>
+      <c r="G35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="2" t="s">
+      <c r="F36" s="8"/>
+      <c r="G36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="2" t="s">
+      <c r="F37" s="8"/>
+      <c r="G37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="2" t="s">
+      <c r="F38" s="8"/>
+      <c r="G38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="2" t="s">
+      <c r="E39" s="7"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="2" t="s">
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="2" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="2" t="s">
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="2" t="s">
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="2" t="s">
+      <c r="E44" s="7"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="2" t="s">
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="2" t="s">
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="2" t="s">
+      <c r="E47" s="7"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="13"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="2" t="s">
+      <c r="E48" s="7"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="2" t="s">
+      <c r="E49" s="7"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="13"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="2" t="s">
+      <c r="E50" s="7"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="2" t="s">
+      <c r="F51" s="8"/>
+      <c r="G51" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="13"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="2" t="s">
+      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H52" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="2" t="s">
+      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:F34"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="E29:F29"/>
@@ -2238,29 +2247,27 @@
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="E40:F40"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:F34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"n/a"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
partial layout of psu
pdn about to look like a mine field
</commit_message>
<xml_diff>
--- a/hardware/MasterBoard_A/Meta.xlsx
+++ b/hardware/MasterBoard_A/Meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\BeeMS\hardware\MasterBoard_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98333C02-14D0-4F61-B223-63F98603464A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AE0B9C-2045-4AE0-8357-7B5949ED0BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{E16E688C-64E3-4955-9FD3-F7092625115C}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="120">
   <si>
     <t>last updated</t>
   </si>
@@ -443,6 +443,18 @@
   </si>
   <si>
     <t>controller CS</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>uart ui</t>
+  </si>
+  <si>
+    <t>uart TX</t>
+  </si>
+  <si>
+    <t>uart RX</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4533B8-A771-42AD-BF13-358F348FDA0F}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:I22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,7 +2047,9 @@
       <c r="D46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="F46" s="8"/>
       <c r="G46" s="1" t="s">
         <v>71</v>
@@ -2057,7 +2071,9 @@
       <c r="D47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="F47" s="8"/>
       <c r="G47" s="1" t="s">
         <v>71</v>
@@ -2079,7 +2095,9 @@
       <c r="D48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="F48" s="8"/>
       <c r="G48" s="1" t="s">
         <v>71</v>
@@ -2201,17 +2219,52 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="E54" s="7"/>
       <c r="F54" s="8"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="G54" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" s="7"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="48">
+    <mergeCell ref="E55:F55"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="E4:E5"/>

</xml_diff>

<commit_message>
up to date meta sheet and made release files
</commit_message>
<xml_diff>
--- a/hardware/MasterBoard_A/Meta.xlsx
+++ b/hardware/MasterBoard_A/Meta.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\BeeMS\hardware\MasterBoard_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AE0B9C-2045-4AE0-8357-7B5949ED0BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E2903C-4796-4E39-8922-82F5431EBEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{E16E688C-64E3-4955-9FD3-F7092625115C}"/>
   </bookViews>
   <sheets>
-    <sheet name="pin planner onboard" sheetId="1" r:id="rId1"/>
+    <sheet name="1.0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="157">
   <si>
     <t>last updated</t>
   </si>
@@ -361,9 +361,6 @@
     <t>SWD</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>SWDIO</t>
   </si>
   <si>
@@ -400,21 +397,9 @@
     <t>PWM bank</t>
   </si>
   <si>
-    <t>bank 1 input 1</t>
-  </si>
-  <si>
     <t>PWM</t>
   </si>
   <si>
-    <t>bank 1 input 2</t>
-  </si>
-  <si>
-    <t>bank 1 input 3</t>
-  </si>
-  <si>
-    <t>bank 1 input 4</t>
-  </si>
-  <si>
     <t>Board side sensing</t>
   </si>
   <si>
@@ -448,13 +433,139 @@
     <t>disabled</t>
   </si>
   <si>
-    <t>uart ui</t>
-  </si>
-  <si>
     <t>uart TX</t>
   </si>
   <si>
-    <t>uart RX</t>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>B14</t>
+  </si>
+  <si>
+    <t>B15</t>
+  </si>
+  <si>
+    <t>B16</t>
+  </si>
+  <si>
+    <t>B17</t>
+  </si>
+  <si>
+    <t>B18</t>
+  </si>
+  <si>
+    <t>B19</t>
+  </si>
+  <si>
+    <t>B20</t>
+  </si>
+  <si>
+    <t>B21</t>
+  </si>
+  <si>
+    <t>B22</t>
+  </si>
+  <si>
+    <t>B23</t>
+  </si>
+  <si>
+    <t>B24</t>
+  </si>
+  <si>
+    <t>B25</t>
+  </si>
+  <si>
+    <t>B26</t>
+  </si>
+  <si>
+    <t>B27</t>
+  </si>
+  <si>
+    <t>B28</t>
+  </si>
+  <si>
+    <t>B29</t>
+  </si>
+  <si>
+    <t>B30</t>
+  </si>
+  <si>
+    <t>B31</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>DIO</t>
+  </si>
+  <si>
+    <t>do not manually configure</t>
+  </si>
+  <si>
+    <t>UART2</t>
+  </si>
+  <si>
+    <t>uart UI</t>
+  </si>
+  <si>
+    <t>UART2 tx</t>
+  </si>
+  <si>
+    <t>UART2 rx</t>
+  </si>
+  <si>
+    <t>bank 1 signal 1</t>
+  </si>
+  <si>
+    <t>bank 1 signal 2</t>
+  </si>
+  <si>
+    <t>bank 1 signal 3</t>
+  </si>
+  <si>
+    <t>bank 1 signal 4</t>
+  </si>
+  <si>
+    <t>reset</t>
   </si>
 </sst>
 </file>
@@ -663,13 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -690,14 +795,62 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1042,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4533B8-A771-42AD-BF13-358F348FDA0F}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,11 +1207,12 @@
     <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="14" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
     <col min="9" max="12" width="9.140625" style="2"/>
-    <col min="13" max="13" width="13.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="2" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1091,47 +1245,54 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="J3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f>IFERROR(INDEX($H$15:$H$1000, MATCH($J3, $G$15:$G$1000, 0)), "n/a")</f>
+        <v>n/a</v>
+      </c>
       <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="M3" s="1" t="str">
-        <f t="shared" ref="M3:M34" si="0">IFERROR(INDEX($H$15:$H$1000, MATCH($L3, $G$15:$G$1000, 0)), "n/a")</f>
+        <f t="shared" ref="K3:M37" si="0">IFERROR(INDEX($H$15:$H$1000, MATCH($L3, $G$15:$G$1000, 0)), "n/a")</f>
         <v>n/a</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="18"/>
+      <c r="H4" s="9"/>
       <c r="L4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1141,12 +1302,12 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1220,7 +1381,7 @@
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>n/a</v>
+        <v>gpio</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1251,7 +1412,7 @@
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>n/a</v>
+        <v>gpio</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1375,45 +1536,45 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
       <c r="L17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+        <v>gpio</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="9" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="18"/>
       <c r="L18" s="1" t="s">
         <v>50</v>
       </c>
@@ -1423,12 +1584,12 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="4" t="s">
         <v>29</v>
       </c>
@@ -1451,7 +1612,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>68</v>
@@ -1459,7 +1620,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
       <c r="G20" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>86</v>
@@ -1544,7 +1705,7 @@
       </c>
       <c r="M23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>n/a</v>
+        <v>UART2 tx</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1569,7 +1730,7 @@
       </c>
       <c r="M24" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>n/a</v>
+        <v>UART2 rx</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1594,7 +1755,7 @@
       </c>
       <c r="M25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>n/a</v>
+        <v>PWM</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1619,7 +1780,7 @@
       </c>
       <c r="M26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>n/a</v>
+        <v>AI</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1638,7 +1799,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
       <c r="G27" s="1" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>86</v>
@@ -1667,7 +1828,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="8"/>
       <c r="G28" s="1" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>86</v>
@@ -1681,14 +1842,26 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="L29" s="1" t="s">
         <v>61</v>
       </c>
@@ -1698,6 +1871,26 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="L30" s="1" t="s">
         <v>62</v>
       </c>
@@ -1716,16 +1909,16 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
       <c r="L32" s="1" t="s">
         <v>64</v>
       </c>
@@ -1735,26 +1928,26 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="18" t="s">
+      <c r="F33" s="13"/>
+      <c r="G33" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H33" s="18"/>
+      <c r="H33" s="9"/>
       <c r="L33" s="1" t="s">
         <v>65</v>
       </c>
@@ -1764,22 +1957,22 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="17"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="15"/>
       <c r="G34" s="4" t="s">
         <v>29</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M34" s="2" t="str">
+      <c r="L34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>gpio</v>
       </c>
@@ -1798,7 +1991,7 @@
         <v>68</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="1" t="s">
@@ -1807,6 +2000,13 @@
       <c r="H35" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="L35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>gpio</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -1822,7 +2022,7 @@
         <v>72</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="1" t="s">
@@ -1831,6 +2031,13 @@
       <c r="H36" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="L36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>gpio</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1840,20 +2047,27 @@
         <v>67</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" s="1" t="s">
         <v>53</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>gpio</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1864,20 +2078,27 @@
         <v>67</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M38" s="1" t="str">
+        <f t="shared" ref="M38:M67" si="1">IFERROR(INDEX($H$15:$H$1000, MATCH($L38, $G$15:$G$1000, 0)), "n/a")</f>
+        <v>n/a</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -1885,10 +2106,10 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>68</v>
@@ -1896,10 +2117,17 @@
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
       <c r="G39" s="1" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>86</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -1907,10 +2135,10 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>68</v>
@@ -1918,10 +2146,17 @@
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
       <c r="G40" s="1" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>86</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -1929,10 +2164,10 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>68</v>
@@ -1940,10 +2175,17 @@
       <c r="E41" s="7"/>
       <c r="F41" s="8"/>
       <c r="G41" s="1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>86</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>gpio</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -1951,10 +2193,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>68</v>
@@ -1962,10 +2204,17 @@
       <c r="E42" s="7"/>
       <c r="F42" s="8"/>
       <c r="G42" s="1" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>86</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -1973,10 +2222,10 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>68</v>
@@ -1984,10 +2233,17 @@
       <c r="E43" s="7"/>
       <c r="F43" s="8"/>
       <c r="G43" s="1" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>86</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -1995,10 +2251,10 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>72</v>
@@ -2006,10 +2262,17 @@
       <c r="E44" s="7"/>
       <c r="F44" s="8"/>
       <c r="G44" s="1" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>86</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M44" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2017,10 +2280,10 @@
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>77</v>
@@ -2028,10 +2291,17 @@
       <c r="E45" s="7"/>
       <c r="F45" s="8"/>
       <c r="G45" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M45" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2039,23 +2309,30 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="1" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2063,23 +2340,30 @@
         <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="1" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M47" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>gpio</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2087,102 +2371,132 @@
         <v>5</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="1" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M48" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="8"/>
       <c r="G49" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M49" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>uart TX</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E50" s="7"/>
+        <v>103</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="F50" s="8"/>
       <c r="G50" s="1" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M50" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>gpio</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>72</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="1" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M51" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>72</v>
@@ -2190,13 +2504,20 @@
       <c r="E52" s="7"/>
       <c r="F52" s="8"/>
       <c r="G52" s="1" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M52" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -2204,7 +2525,7 @@
         <v>17</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>72</v>
@@ -2212,58 +2533,225 @@
       <c r="E53" s="7"/>
       <c r="F53" s="8"/>
       <c r="G53" s="1" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L53" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M53" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E54" s="7"/>
       <c r="F54" s="8"/>
       <c r="G54" s="1" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M54" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
       <c r="E55" s="7"/>
       <c r="F55" s="8"/>
-      <c r="G55" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="L55" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M55" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="L56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M56" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="L57" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M57" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="L58" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M58" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L59" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M59" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L60" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M60" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>gpio</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L61" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M61" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>gpio</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L62" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M62" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L63" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="M63" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M64" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="65" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L65" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M65" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="66" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+    </row>
+    <row r="67" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="52">
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:F34"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
@@ -2280,47 +2768,20 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:F34"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M34">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"n/a"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
up to date meta sheet
excel save prompt was hiding behind other tabs D:
</commit_message>
<xml_diff>
--- a/hardware/MasterBoard_A/Meta.xlsx
+++ b/hardware/MasterBoard_A/Meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\BeeMS\hardware\MasterBoard_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E2903C-4796-4E39-8922-82F5431EBEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1A04B7-FB38-479F-AE88-7CEC65B35E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{E16E688C-64E3-4955-9FD3-F7092625115C}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="160">
   <si>
     <t>last updated</t>
   </si>
@@ -566,6 +566,15 @@
   </si>
   <si>
     <t>reset</t>
+  </si>
+  <si>
+    <t>parts ordered from mouser</t>
+  </si>
+  <si>
+    <t>tracking #</t>
+  </si>
+  <si>
+    <t>1Z7759450314578199</t>
   </si>
 </sst>
 </file>
@@ -748,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -804,39 +813,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1195,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4533B8-A771-42AD-BF13-358F348FDA0F}">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,15 +1197,17 @@
     <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
     <col min="9" max="12" width="9.140625" style="2"/>
     <col min="13" max="13" width="20.5703125" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="14" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="13.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>46011</v>
+        <v>46016</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1234,8 +1220,13 @@
       <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1243,8 +1234,14 @@
         <f>IFERROR(INDEX($H$15:$H$1000, MATCH($L2, $G$15:$G$1000, 0)), "n/a")</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
@@ -1270,7 +1267,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1301,7 +1298,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="11"/>
       <c r="C5" s="9"/>
@@ -1322,7 +1319,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1353,7 +1350,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1384,7 +1381,7 @@
         <v>gpio</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1415,7 +1412,7 @@
         <v>gpio</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1432,7 +1429,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1449,7 +1446,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1466,7 +1463,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1483,7 +1480,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1500,7 +1497,7 @@
         <v>n/a</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1517,7 +1514,7 @@
         <v>spi0 SCLK</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L15" s="1" t="s">
         <v>47</v>
       </c>
@@ -1526,7 +1523,7 @@
         <v>spi0 MISO/POCI</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2715,7 +2712,8 @@
       <c r="M67" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="53">
+    <mergeCell ref="O1:Q1"/>
     <mergeCell ref="E56:F56"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="E58:F58"/>
@@ -2771,17 +2769,17 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>